<commit_message>
rerun with v12 hist
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -14,8 +14,8 @@
     <sheet name="Craniopharyngioma" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="ATRT" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Meningioma" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Mesenchymal tumor" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="DIPG or DMG" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="DIPG or DMG" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Mesenchymal tumor" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Neurofibroma plexiform" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="Non-neoplastic tumor" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Germ cell tumor" sheetId="13" state="visible" r:id="rId13"/>
@@ -434,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.159853986764841</v>
+        <v>0.15230869731919</v>
       </c>
     </row>
     <row r="3">
@@ -456,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.591169994627452</v>
+        <v>0.7931779162466</v>
       </c>
     </row>
     <row r="5">
@@ -489,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.895178412788497</v>
+        <v>0.869185449350616</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +500,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.606117887026658</v>
+        <v>0.62685469729387</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.617006964935405</v>
+        <v>0.76454731048697</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.142842410000663</v>
+        <v>0.681940144478844</v>
       </c>
     </row>
     <row r="3">
@@ -558,7 +558,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.999999999999984</v>
+        <v>0.284829721362229</v>
       </c>
     </row>
     <row r="4">
@@ -569,7 +569,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.999999999999978</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -580,7 +580,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.999999999999977</v>
+        <v>0.508771929824559</v>
       </c>
     </row>
     <row r="6">
@@ -591,7 +591,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.999999999999989</v>
+        <v>0.999999999999994</v>
       </c>
     </row>
     <row r="7">
@@ -602,7 +602,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.892403831447009</v>
+        <v>0.733266733266733</v>
       </c>
     </row>
     <row r="8">
@@ -613,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.364672364672365</v>
+        <v>0.0759240759240759</v>
       </c>
     </row>
     <row r="9">
@@ -624,7 +624,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.864541367693624</v>
+        <v>0.635711125445117</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.297702297702298</v>
       </c>
     </row>
     <row r="3">
@@ -773,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3889785729145</v>
+        <v>0.422874973996255</v>
       </c>
     </row>
     <row r="3">
@@ -784,7 +784,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.659246931558144</v>
       </c>
     </row>
     <row r="4">
@@ -795,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.419446640316208</v>
+        <v>0.564584980237159</v>
       </c>
     </row>
     <row r="5">
@@ -806,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.568306476132566</v>
+        <v>0.564584980237159</v>
       </c>
     </row>
     <row r="6">
@@ -817,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.419446640316208</v>
+        <v>0.564584980237159</v>
       </c>
     </row>
     <row r="7">
@@ -828,7 +828,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.263486513486514</v>
+        <v>0.43956043956044</v>
       </c>
     </row>
     <row r="8">
@@ -850,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.151460181035003</v>
+        <v>0.278072325213818</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +999,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.372727272727273</v>
+        <v>0.33006993006993</v>
       </c>
     </row>
     <row r="3">
@@ -1225,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.324455022174711</v>
+        <v>0.387996466662305</v>
       </c>
     </row>
     <row r="3">
@@ -1236,7 +1236,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.379171301446051</v>
+        <v>0.389108813714585</v>
       </c>
     </row>
     <row r="4">
@@ -1247,7 +1247,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.288148447770254</v>
+        <v>0.275804815808414</v>
       </c>
     </row>
     <row r="5">
@@ -1258,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.999999999999999</v>
+        <v>0.999999999999982</v>
       </c>
     </row>
     <row r="6">
@@ -1269,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.769744160177982</v>
+        <v>0.762971929594966</v>
       </c>
     </row>
     <row r="7">
@@ -1280,7 +1280,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.657592598096031</v>
+        <v>0.721120984278879</v>
       </c>
     </row>
     <row r="8">
@@ -1291,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.707717911379239</v>
+        <v>0.626081012808702</v>
       </c>
     </row>
     <row r="9">
@@ -1302,7 +1302,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.723730448233365</v>
+        <v>0.403692093453513</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0189441240387239</v>
+        <v>0.0231617439105454</v>
       </c>
     </row>
     <row r="8">
@@ -1451,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.438889237590421</v>
+        <v>0.511414611707042</v>
       </c>
     </row>
     <row r="3">
@@ -1462,7 +1462,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0366833689908165</v>
+        <v>0.0191251203686029</v>
       </c>
     </row>
     <row r="4">
@@ -1473,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.795106016808421</v>
+        <v>0.830125478641495</v>
       </c>
     </row>
     <row r="5">
@@ -1484,7 +1484,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.563609097392122</v>
+        <v>0.608353352840895</v>
       </c>
     </row>
     <row r="6">
@@ -1495,7 +1495,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.501341962501177</v>
+        <v>0.532508089844862</v>
       </c>
     </row>
     <row r="7">
@@ -1506,7 +1506,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.167648024835945</v>
+        <v>0.190274200316843</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.153764736927889</v>
+        <v>0.193583517235016</v>
       </c>
     </row>
     <row r="9">
@@ -1528,7 +1528,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.97664153065597</v>
+        <v>0.367827062567279</v>
       </c>
     </row>
   </sheetData>
@@ -1564,7 +1564,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0504391183087111</v>
+        <v>0.0485949954198866</v>
       </c>
     </row>
     <row r="3">
@@ -1586,7 +1586,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.161350632737374</v>
+        <v>0.357593243242194</v>
       </c>
     </row>
     <row r="5">
@@ -1597,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.222734188821585</v>
+        <v>0.212651737225106</v>
       </c>
     </row>
     <row r="6">
@@ -1608,7 +1608,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.38808983464961</v>
+        <v>0.384467290382669</v>
       </c>
     </row>
     <row r="7">
@@ -1619,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.241976892260026</v>
+        <v>0.212297500884979</v>
       </c>
     </row>
     <row r="8">
@@ -1630,7 +1630,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0307038580733801</v>
+        <v>0.0335746893173699</v>
       </c>
     </row>
     <row r="9">
@@ -1641,7 +1641,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.398573745812535</v>
+        <v>0.768522422425236</v>
       </c>
     </row>
   </sheetData>
@@ -1677,7 +1677,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0958458050500238</v>
+        <v>0.197737271253414</v>
       </c>
     </row>
     <row r="3">
@@ -1688,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.156123041889036</v>
+        <v>0.0860576559380436</v>
       </c>
     </row>
     <row r="4">
@@ -1699,7 +1699,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.740068553056341</v>
+        <v>0.796815847884649</v>
       </c>
     </row>
     <row r="5">
@@ -1710,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.79475648318652</v>
+        <v>0.844003973383851</v>
       </c>
     </row>
     <row r="6">
@@ -1721,7 +1721,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.633241713303095</v>
+        <v>0.999999999999984</v>
       </c>
     </row>
     <row r="7">
@@ -1732,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.452196610419698</v>
+        <v>0.442905776000836</v>
       </c>
     </row>
     <row r="8">
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.735101548656599</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1754,7 +1754,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.695936771177664</v>
+        <v>0.299113352181795</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1812,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.608819345661452</v>
+        <v>0.644381223328592</v>
       </c>
     </row>
     <row r="5">
@@ -2129,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.819814241486068</v>
+        <v>0.0791739604170237</v>
       </c>
     </row>
     <row r="3">
@@ -2140,7 +2140,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.284829721362229</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -2151,7 +2151,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.746180752659459</v>
       </c>
     </row>
     <row r="5">
@@ -2162,7 +2162,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.508771929824559</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -2173,7 +2173,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.999999999999994</v>
+        <v>0.907161981862534</v>
       </c>
     </row>
     <row r="7">
@@ -2184,7 +2184,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.733266733266733</v>
+        <v>0.344182227681443</v>
       </c>
     </row>
     <row r="8">
@@ -2195,7 +2195,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0759240759240759</v>
+        <v>0.613245356793744</v>
       </c>
     </row>
     <row r="9">
@@ -2206,7 +2206,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.635711125445117</v>
+        <v>0.00457730524302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun with correct plot groups
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -1677,7 +1677,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.197737271253414</v>
+        <v>0.0874616484567612</v>
       </c>
     </row>
     <row r="3">
@@ -1688,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0860576559380436</v>
+        <v>0.0722971792396567</v>
       </c>
     </row>
     <row r="4">
@@ -1699,7 +1699,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.796815847884649</v>
+        <v>0.632646633329443</v>
       </c>
     </row>
     <row r="5">
@@ -1710,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.844003973383851</v>
+        <v>0.747469115830449</v>
       </c>
     </row>
     <row r="6">
@@ -1721,7 +1721,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.999999999999984</v>
+        <v>0.765044002655438</v>
       </c>
     </row>
     <row r="7">
@@ -1732,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.442905776000836</v>
+        <v>0.688070088451452</v>
       </c>
     </row>
     <row r="8">
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0.806157348933911</v>
       </c>
     </row>
     <row r="9">
@@ -1754,7 +1754,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.299113352181795</v>
+        <v>0.831034212389158</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0791739604170237</v>
+        <v>0.158302905892242</v>
       </c>
     </row>
     <row r="3">
@@ -2140,7 +2140,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0.99999999999995</v>
       </c>
     </row>
     <row r="4">
@@ -2151,7 +2151,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.746180752659459</v>
+        <v>0.999999999999968</v>
       </c>
     </row>
     <row r="5">
@@ -2173,7 +2173,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.907161981862534</v>
+        <v>0.862159087147157</v>
       </c>
     </row>
     <row r="7">
@@ -2184,7 +2184,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.344182227681443</v>
+        <v>0.895123569422763</v>
       </c>
     </row>
     <row r="8">
@@ -2195,7 +2195,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.613245356793744</v>
+        <v>0.338624338624339</v>
       </c>
     </row>
     <row r="9">
@@ -2206,7 +2206,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00457730524302</v>
+        <v>0.574228093777768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun with updated survival
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -489,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.869185449350616</v>
+        <v>0.931888656937515</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +500,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.62685469729387</v>
+        <v>0.667171970824453</v>
       </c>
     </row>
     <row r="9">
@@ -602,7 +602,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.733266733266733</v>
+        <v>0.635364635364635</v>
       </c>
     </row>
     <row r="8">
@@ -828,7 +828,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.43956043956044</v>
+        <v>0.367632367632368</v>
       </c>
     </row>
     <row r="8">
@@ -1280,7 +1280,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.721120984278879</v>
+        <v>0.679119715982637</v>
       </c>
     </row>
     <row r="8">
@@ -1291,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.626081012808702</v>
+        <v>0.679119715982637</v>
       </c>
     </row>
     <row r="9">
@@ -1393,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0231617439105454</v>
+        <v>0.0161437336988245</v>
       </c>
     </row>
     <row r="8">
@@ -1404,7 +1404,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0212641706024715</v>
+        <v>0.0186637927222251</v>
       </c>
     </row>
     <row r="9">
@@ -1619,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.212297500884979</v>
+        <v>0.323974445713471</v>
       </c>
     </row>
     <row r="8">
@@ -1630,7 +1630,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0335746893173699</v>
+        <v>0.0451638578585793</v>
       </c>
     </row>
     <row r="9">
@@ -1732,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.688070088451452</v>
+        <v>0.494581501411332</v>
       </c>
     </row>
     <row r="8">
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.806157348933911</v>
+        <v>0.82858453483385</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
update script code, rerun module
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -434,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.15230869731919</v>
+        <v>0.083541683621774</v>
       </c>
     </row>
     <row r="3">
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00697142824782929</v>
+        <v>0.0204091723342268</v>
       </c>
     </row>
     <row r="4">
@@ -456,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7931779162466</v>
+        <v>0.86626745181243</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.42129588393458</v>
+        <v>0.588174611595652</v>
       </c>
     </row>
     <row r="6">
@@ -478,7 +478,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.260193091816979</v>
+        <v>0.276767428792189</v>
       </c>
     </row>
     <row r="7">
@@ -489,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.931888656937515</v>
+        <v>0.721643318278074</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +500,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.667171970824453</v>
+        <v>0.326402980186976</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.76454731048697</v>
+        <v>0.464613053587257</v>
       </c>
     </row>
   </sheetData>
@@ -624,7 +624,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.635711125445117</v>
+        <v>0.924520737821253</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +737,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.135346095457142</v>
+        <v>0.646990031211512</v>
       </c>
     </row>
   </sheetData>
@@ -850,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.278072325213818</v>
+        <v>0.125156485427265</v>
       </c>
     </row>
   </sheetData>
@@ -886,7 +886,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.573426573426573</v>
+        <v>0.148251748251748</v>
       </c>
     </row>
     <row r="3">
@@ -908,7 +908,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.622377622377623</v>
+        <v>0.647552447552448</v>
       </c>
     </row>
     <row r="5">
@@ -919,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.706293706293707</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -941,7 +941,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.863636363636364</v>
+        <v>0.367676767676768</v>
       </c>
     </row>
     <row r="8">
@@ -952,7 +952,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.281818181818182</v>
+        <v>0.214141414141414</v>
       </c>
     </row>
     <row r="9">
@@ -963,7 +963,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.283722698873285</v>
+        <v>0.428523908344215</v>
       </c>
     </row>
   </sheetData>
@@ -1076,7 +1076,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.348247079876413</v>
+        <v>0.0600624085865772</v>
       </c>
     </row>
   </sheetData>
@@ -1112,7 +1112,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.335901027077498</v>
+        <v>0.645098039215686</v>
       </c>
     </row>
     <row r="3">
@@ -1123,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.101307189542484</v>
+        <v>0.119281045751634</v>
       </c>
     </row>
     <row r="4">
@@ -1156,7 +1156,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.999999999999995</v>
+        <v>0.999999999999997</v>
       </c>
     </row>
     <row r="7">
@@ -1167,7 +1167,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.335216993395542</v>
+        <v>0.903408211942422</v>
       </c>
     </row>
     <row r="8">
@@ -1178,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0897435897435898</v>
+        <v>0.261538461538462</v>
       </c>
     </row>
     <row r="9">
@@ -1189,7 +1189,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.81155501740346</v>
+        <v>0.283319589457907</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.387996466662305</v>
+        <v>0.100858857941891</v>
       </c>
     </row>
     <row r="3">
@@ -1236,7 +1236,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.389108813714585</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1247,7 +1247,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.275804815808414</v>
+        <v>0.490904927043123</v>
       </c>
     </row>
     <row r="5">
@@ -1258,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.999999999999982</v>
+        <v>0.75044100628083</v>
       </c>
     </row>
     <row r="6">
@@ -1269,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.762971929594966</v>
+        <v>0.665568860098732</v>
       </c>
     </row>
     <row r="7">
@@ -1280,7 +1280,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.679119715982637</v>
+        <v>0.930353912409497</v>
       </c>
     </row>
     <row r="8">
@@ -1291,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.679119715982637</v>
+        <v>0.838406383109114</v>
       </c>
     </row>
     <row r="9">
@@ -1302,7 +1302,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.403692093453513</v>
+        <v>0.596430178913545</v>
       </c>
     </row>
   </sheetData>
@@ -1338,7 +1338,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.311501761161828</v>
+        <v>0.717032215421925</v>
       </c>
     </row>
     <row r="3">
@@ -1349,7 +1349,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.611411770823126</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1360,7 +1360,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.826989698111794</v>
+        <v>0.987148764481946</v>
       </c>
     </row>
     <row r="5">
@@ -1371,7 +1371,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.959984730439822</v>
+        <v>0.971304078866354</v>
       </c>
     </row>
     <row r="6">
@@ -1382,7 +1382,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.999999999999983</v>
+        <v>0.638240668305458</v>
       </c>
     </row>
     <row r="7">
@@ -1393,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0161437336988245</v>
+        <v>0.0215000581483138</v>
       </c>
     </row>
     <row r="8">
@@ -1404,7 +1404,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0186637927222251</v>
+        <v>0.0136864060128698</v>
       </c>
     </row>
     <row r="9">
@@ -1415,7 +1415,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.730130453857582</v>
+        <v>0.824486303633589</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.511414611707042</v>
+        <v>0.462739122413669</v>
       </c>
     </row>
     <row r="3">
@@ -1462,7 +1462,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0191251203686029</v>
+        <v>0.0578532713191215</v>
       </c>
     </row>
     <row r="4">
@@ -1473,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.830125478641495</v>
+        <v>0.999999999999986</v>
       </c>
     </row>
     <row r="5">
@@ -1484,7 +1484,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.608353352840895</v>
+        <v>0.656580631831596</v>
       </c>
     </row>
     <row r="6">
@@ -1495,7 +1495,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.532508089844862</v>
+        <v>0.999999999999963</v>
       </c>
     </row>
     <row r="7">
@@ -1506,7 +1506,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.190274200316843</v>
+        <v>0.336867791184883</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.193583517235016</v>
+        <v>0.499350846186132</v>
       </c>
     </row>
     <row r="9">
@@ -1528,7 +1528,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.367827062567279</v>
+        <v>0.943625773616395</v>
       </c>
     </row>
   </sheetData>
@@ -1564,7 +1564,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0485949954198866</v>
+        <v>0.220196207956647</v>
       </c>
     </row>
     <row r="3">
@@ -1586,7 +1586,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.357593243242194</v>
+        <v>0.72429431453387</v>
       </c>
     </row>
     <row r="5">
@@ -1597,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.212651737225106</v>
+        <v>0.450754898244027</v>
       </c>
     </row>
     <row r="6">
@@ -1608,7 +1608,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.384467290382669</v>
+        <v>0.830379412511969</v>
       </c>
     </row>
     <row r="7">
@@ -1619,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.323974445713471</v>
+        <v>0.169620654830765</v>
       </c>
     </row>
     <row r="8">
@@ -1630,7 +1630,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0451638578585793</v>
+        <v>0.146688186321032</v>
       </c>
     </row>
     <row r="9">
@@ -1641,7 +1641,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.768522422425236</v>
+        <v>0.872589914881906</v>
       </c>
     </row>
   </sheetData>
@@ -1677,7 +1677,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0874616484567612</v>
+        <v>0.0549812456875758</v>
       </c>
     </row>
     <row r="3">
@@ -1688,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0722971792396567</v>
+        <v>0.0580535500081479</v>
       </c>
     </row>
     <row r="4">
@@ -1699,7 +1699,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.632646633329443</v>
+        <v>0.398228106546933</v>
       </c>
     </row>
     <row r="5">
@@ -1710,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.747469115830449</v>
+        <v>0.618892857690358</v>
       </c>
     </row>
     <row r="6">
@@ -1721,7 +1721,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.765044002655438</v>
+        <v>0.55188821452344</v>
       </c>
     </row>
     <row r="7">
@@ -1732,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.494581501411332</v>
+        <v>0.516918809678844</v>
       </c>
     </row>
     <row r="8">
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.82858453483385</v>
+        <v>0.886473974807497</v>
       </c>
     </row>
     <row r="9">
@@ -1754,7 +1754,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.831034212389158</v>
+        <v>0.967326029074045</v>
       </c>
     </row>
   </sheetData>
@@ -1790,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0600739548107969</v>
+        <v>0.59919028340081</v>
       </c>
     </row>
     <row r="3">
@@ -1801,7 +1801,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0660295923453818</v>
+        <v>0.255060728744939</v>
       </c>
     </row>
     <row r="4">
@@ -1812,7 +1812,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.644381223328592</v>
+        <v>0.999999999999995</v>
       </c>
     </row>
     <row r="5">
@@ -1823,7 +1823,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.715504978662871</v>
       </c>
     </row>
     <row r="6">
@@ -1845,7 +1845,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.580241935483871</v>
+        <v>0.907258064516129</v>
       </c>
     </row>
     <row r="8">
@@ -1856,7 +1856,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.383064516129032</v>
+        <v>0.326612903225806</v>
       </c>
     </row>
     <row r="9">
@@ -1867,7 +1867,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.173936963364681</v>
+        <v>0.229161113594648</v>
       </c>
     </row>
   </sheetData>
@@ -1903,7 +1903,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.979266916658221</v>
+        <v>0.432655369039808</v>
       </c>
     </row>
     <row r="3">
@@ -1914,7 +1914,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.677616747181965</v>
+        <v>0.694584286803966</v>
       </c>
     </row>
     <row r="4">
@@ -1925,7 +1925,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.705442383703247</v>
+        <v>0.455413419532409</v>
       </c>
     </row>
     <row r="5">
@@ -1936,7 +1936,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.490390189520623</v>
+        <v>0.169836296426685</v>
       </c>
     </row>
     <row r="6">
@@ -1947,7 +1947,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.447863247863246</v>
+        <v>0.511794871794871</v>
       </c>
     </row>
     <row r="7">
@@ -1958,7 +1958,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.80668256228897</v>
+        <v>0.219796130642813</v>
       </c>
     </row>
     <row r="8">
@@ -1969,7 +1969,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.891890352210719</v>
+        <v>0.28717351298587</v>
       </c>
     </row>
     <row r="9">
@@ -1980,7 +1980,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.100366402248816</v>
+        <v>0.288619115786948</v>
       </c>
     </row>
   </sheetData>
@@ -2093,7 +2093,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.738273151589412</v>
+        <v>0.094779946136451</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.158302905892242</v>
+        <v>0.515458449661513</v>
       </c>
     </row>
     <row r="3">
@@ -2162,7 +2162,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.844026805515887</v>
       </c>
     </row>
     <row r="6">
@@ -2184,7 +2184,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.895123569422763</v>
+        <v>0.449023462236327</v>
       </c>
     </row>
     <row r="8">
@@ -2195,7 +2195,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.338624338624339</v>
+        <v>0.124542124542125</v>
       </c>
     </row>
     <row r="9">
@@ -2206,7 +2206,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.574228093777768</v>
+        <v>0.830698294656258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun module with updated hist,plp,survival
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -434,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.083541683621774</v>
+        <v>0.0916255274919478</v>
       </c>
     </row>
     <row r="3">
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0204091723342268</v>
+        <v>0.0204667639867541</v>
       </c>
     </row>
     <row r="4">
@@ -456,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.86626745181243</v>
+        <v>0.876575011907386</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.588174611595652</v>
+        <v>0.590007509317855</v>
       </c>
     </row>
     <row r="6">
@@ -478,7 +478,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.276767428792189</v>
+        <v>0.278667237227906</v>
       </c>
     </row>
     <row r="7">
@@ -489,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.721643318278074</v>
+        <v>0.653398128943485</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +500,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.326402980186976</v>
+        <v>0.325126774991726</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.464613053587257</v>
+        <v>0.114380406814406</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0215000581483138</v>
+        <v>0.0122612056281556</v>
       </c>
     </row>
     <row r="8">
@@ -1404,7 +1404,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0136864060128698</v>
+        <v>0.00899774600656136</v>
       </c>
     </row>
     <row r="9">
@@ -1451,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.462739122413669</v>
+        <v>0.444612451662848</v>
       </c>
     </row>
     <row r="3">
@@ -1462,7 +1462,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0578532713191215</v>
+        <v>0.0568379519357277</v>
       </c>
     </row>
     <row r="4">
@@ -1473,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.999999999999986</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1484,7 +1484,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.656580631831596</v>
+        <v>0.649435849758916</v>
       </c>
     </row>
     <row r="6">
@@ -1495,7 +1495,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.999999999999963</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1506,7 +1506,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.336867791184883</v>
+        <v>0.327767463046345</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.499350846186132</v>
+        <v>0.507288935909022</v>
       </c>
     </row>
     <row r="9">
@@ -1528,7 +1528,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.943625773616395</v>
+        <v>0.0488695670927194</v>
       </c>
     </row>
   </sheetData>
@@ -1677,7 +1677,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0549812456875758</v>
+        <v>0.0151928813071579</v>
       </c>
     </row>
     <row r="3">
@@ -1688,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0580535500081479</v>
+        <v>0.106820568787808</v>
       </c>
     </row>
     <row r="4">
@@ -1699,7 +1699,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.398228106546933</v>
+        <v>0.571152892328409</v>
       </c>
     </row>
     <row r="5">
@@ -1721,7 +1721,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.55188821452344</v>
+        <v>0.504555722356751</v>
       </c>
     </row>
     <row r="7">
@@ -1732,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.516918809678844</v>
+        <v>0.373852037579399</v>
       </c>
     </row>
     <row r="8">
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.886473974807497</v>
+        <v>0.700701203497786</v>
       </c>
     </row>
     <row r="9">
@@ -1754,7 +1754,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.967326029074045</v>
+        <v>0.632726822660118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun module w updated plp
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -489,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.653398128943485</v>
+        <v>0.658631193852452</v>
       </c>
     </row>
     <row r="8">
@@ -511,7 +511,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.114380406814406</v>
+        <v>0.0809511288726465</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0122612056281556</v>
+        <v>0.0112805347433453</v>
       </c>
     </row>
     <row r="8">
@@ -1506,7 +1506,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.327767463046345</v>
+        <v>0.304722764052948</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.507288935909022</v>
+        <v>0.490780770910609</v>
       </c>
     </row>
     <row r="9">
@@ -1903,7 +1903,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.432655369039808</v>
+        <v>0.696434129477608</v>
       </c>
     </row>
     <row r="3">
@@ -1914,7 +1914,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.694584286803966</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1925,7 +1925,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.455413419532409</v>
+        <v>0.705442383703247</v>
       </c>
     </row>
     <row r="5">
@@ -1936,7 +1936,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.169836296426685</v>
+        <v>0.490390189520623</v>
       </c>
     </row>
     <row r="6">
@@ -1947,7 +1947,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.511794871794871</v>
+        <v>0.447863247863246</v>
       </c>
     </row>
     <row r="7">
@@ -1958,7 +1958,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.219796130642813</v>
+        <v>0.260831159686995</v>
       </c>
     </row>
     <row r="8">
@@ -1969,7 +1969,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.28717351298587</v>
+        <v>0.285246835544318</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
rerun with new APC variants
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -434,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0916255274919478</v>
+        <v>0.0896185966222548</v>
       </c>
     </row>
     <row r="3">
@@ -445,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0204667639867541</v>
+        <v>0.0208619595159617</v>
       </c>
     </row>
     <row r="4">
@@ -456,7 +456,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.876575011907386</v>
+        <v>0.90258835020493</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.590007509317855</v>
+        <v>0.617880140186009</v>
       </c>
     </row>
     <row r="6">
@@ -478,7 +478,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.278667237227906</v>
+        <v>0.276767428792189</v>
       </c>
     </row>
     <row r="7">
@@ -489,7 +489,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.658631193852452</v>
+        <v>0.732449677492432</v>
       </c>
     </row>
     <row r="8">
@@ -500,7 +500,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.325126774991726</v>
+        <v>0.282133084993859</v>
       </c>
     </row>
     <row r="9">
@@ -511,7 +511,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0809511288726465</v>
+        <v>0.284369753577153</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.422874973996255</v>
+        <v>0.533238741934394</v>
       </c>
     </row>
     <row r="3">
@@ -784,7 +784,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.659246931558144</v>
+        <v>0.408212560386474</v>
       </c>
     </row>
     <row r="4">
@@ -795,7 +795,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.564584980237159</v>
+        <v>0.282003986351813</v>
       </c>
     </row>
     <row r="5">
@@ -806,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.564584980237159</v>
+        <v>0.615904868078785</v>
       </c>
     </row>
     <row r="6">
@@ -817,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.564584980237159</v>
+        <v>0.231809736157562</v>
       </c>
     </row>
     <row r="7">
@@ -850,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.125156485427265</v>
+        <v>0.353287117317915</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.100858857941891</v>
+        <v>0.0907981961597089</v>
       </c>
     </row>
     <row r="3">
@@ -1247,7 +1247,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.490904927043123</v>
+        <v>0.426613045834412</v>
       </c>
     </row>
     <row r="5">
@@ -1258,7 +1258,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.75044100628083</v>
+        <v>0.81427569093866</v>
       </c>
     </row>
     <row r="6">
@@ -1269,7 +1269,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.665568860098732</v>
+        <v>0.780633752602614</v>
       </c>
     </row>
     <row r="7">
@@ -1280,7 +1280,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.930353912409497</v>
+        <v>0.878298596491423</v>
       </c>
     </row>
     <row r="8">
@@ -1291,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.838406383109114</v>
+        <v>0.759361447436373</v>
       </c>
     </row>
     <row r="9">
@@ -1302,7 +1302,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.596430178913545</v>
+        <v>0.739996268959378</v>
       </c>
     </row>
   </sheetData>
@@ -1338,7 +1338,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.717032215421925</v>
+        <v>0.713705357283287</v>
       </c>
     </row>
     <row r="3">
@@ -1360,7 +1360,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.987148764481946</v>
+        <v>0.987141116454481</v>
       </c>
     </row>
     <row r="5">
@@ -1371,7 +1371,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.971304078866354</v>
+        <v>0.946801804848752</v>
       </c>
     </row>
     <row r="6">
@@ -1382,7 +1382,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.638240668305458</v>
+        <v>0.639519327674786</v>
       </c>
     </row>
     <row r="7">
@@ -1393,7 +1393,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0112805347433453</v>
+        <v>0.00369227398780271</v>
       </c>
     </row>
     <row r="8">
@@ -1404,7 +1404,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00899774600656136</v>
+        <v>0.0034650073118416</v>
       </c>
     </row>
     <row r="9">
@@ -1415,7 +1415,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.824486303633589</v>
+        <v>0.0878796824057952</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.444612451662848</v>
+        <v>0.498965426816437</v>
       </c>
     </row>
     <row r="3">
@@ -1462,7 +1462,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0568379519357277</v>
+        <v>0.0565098418868229</v>
       </c>
     </row>
     <row r="4">
@@ -1473,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.999999999999979</v>
       </c>
     </row>
     <row r="5">
@@ -1484,7 +1484,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.649435849758916</v>
+        <v>0.631203160659328</v>
       </c>
     </row>
     <row r="6">
@@ -1495,7 +1495,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0.999999999999973</v>
       </c>
     </row>
     <row r="7">
@@ -1506,7 +1506,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304722764052948</v>
+        <v>0.23832192708036</v>
       </c>
     </row>
     <row r="8">
@@ -1517,7 +1517,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.490780770910609</v>
+        <v>0.419110881762562</v>
       </c>
     </row>
     <row r="9">
@@ -1528,7 +1528,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0488695670927194</v>
+        <v>0.167425229268679</v>
       </c>
     </row>
   </sheetData>
@@ -1564,7 +1564,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.220196207956647</v>
+        <v>0.233152960277338</v>
       </c>
     </row>
     <row r="3">
@@ -1586,7 +1586,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.72429431453387</v>
+        <v>0.576531536291638</v>
       </c>
     </row>
     <row r="5">
@@ -1597,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.450754898244027</v>
+        <v>0.368336454051302</v>
       </c>
     </row>
     <row r="6">
@@ -1608,7 +1608,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.830379412511969</v>
+        <v>0.8325789171934</v>
       </c>
     </row>
     <row r="7">
@@ -1619,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.169620654830765</v>
+        <v>0.154349260156668</v>
       </c>
     </row>
     <row r="8">
@@ -1630,7 +1630,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.146688186321032</v>
+        <v>0.144877451159352</v>
       </c>
     </row>
     <row r="9">
@@ -1641,7 +1641,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.872589914881906</v>
+        <v>0.147476037454092</v>
       </c>
     </row>
   </sheetData>
@@ -1677,7 +1677,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0151928813071579</v>
+        <v>0.0625772201692652</v>
       </c>
     </row>
     <row r="3">
@@ -1688,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>0.106820568787808</v>
+        <v>0.116505436478945</v>
       </c>
     </row>
     <row r="4">
@@ -1699,7 +1699,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.571152892328409</v>
+        <v>0.35325139146675</v>
       </c>
     </row>
     <row r="5">
@@ -1710,7 +1710,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.618892857690358</v>
+        <v>0.575562395767317</v>
       </c>
     </row>
     <row r="6">
@@ -1721,7 +1721,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.504555722356751</v>
+        <v>0.402895113668335</v>
       </c>
     </row>
     <row r="7">
@@ -1732,7 +1732,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>0.373852037579399</v>
+        <v>0.516918809678844</v>
       </c>
     </row>
     <row r="8">
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>0.700701203497786</v>
+        <v>0.886473974807497</v>
       </c>
     </row>
     <row r="9">
@@ -1754,7 +1754,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="n">
-        <v>0.632726822660118</v>
+        <v>0.201167318853901</v>
       </c>
     </row>
   </sheetData>
@@ -2173,7 +2173,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0.862159087147157</v>
+        <v>0.999999999999972</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
rm excel output rownames
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t xml:space="preserve"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">term</t>
   </si>
@@ -38,49 +35,25 @@
     <t xml:space="preserve">pvalue</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">sex</t>
   </si>
   <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
     <t xml:space="preserve">race</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
   </si>
   <si>
     <t xml:space="preserve">ancestry</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
     <t xml:space="preserve">ethnicity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
   </si>
   <si>
     <t xml:space="preserve">OS_years</t>
   </si>
   <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
     <t xml:space="preserve">EFS_years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
   </si>
   <si>
     <t xml:space="preserve">tmb</t>
@@ -422,95 +395,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.0896185966222548</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.0208619595159617</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.90258835020493</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.617880140186009</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.276767428792189</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.732449677492432</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.282133084993859</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.284369753577153</v>
       </c>
     </row>
@@ -535,95 +481,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.681940144478844</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.284829721362229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.508771929824559</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.999999999999994</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.635364635364635</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.0759240759240759</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.924520737821253</v>
       </c>
     </row>
@@ -648,95 +567,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.297702297702298</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.604395604395606</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.503496503496504</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.33006993006993</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.646990031211512</v>
       </c>
     </row>
@@ -761,95 +653,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.533238741934394</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.408212560386474</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.282003986351813</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.615904868078785</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.231809736157562</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.367632367632368</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.635364635364635</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.353287117317915</v>
       </c>
     </row>
@@ -874,95 +739,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.148251748251748</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.647552447552448</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.367676767676768</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.214141414141414</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.428523908344215</v>
       </c>
     </row>
@@ -987,95 +825,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.33006993006993</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.664335664335665</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.328671328671329</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.111111111111111</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.666666666666667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.0600624085865772</v>
       </c>
     </row>
@@ -1100,95 +911,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.645098039215686</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.119281045751634</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.999999999999997</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.903408211942422</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.261538461538462</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.283319589457907</v>
       </c>
     </row>
@@ -1213,95 +997,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.0907981961597089</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.426613045834412</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.81427569093866</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.780633752602614</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.878298596491423</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.759361447436373</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.739996268959378</v>
       </c>
     </row>
@@ -1326,95 +1083,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.713705357283287</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.987141116454481</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.946801804848752</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.639519327674786</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.00369227398780271</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.0034650073118416</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.0878796824057952</v>
       </c>
     </row>
@@ -1439,95 +1169,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.498965426816437</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.0565098418868229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.999999999999979</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.631203160659328</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.999999999999973</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.23832192708036</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.419110881762562</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.167425229268679</v>
       </c>
     </row>
@@ -1552,95 +1255,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.233152960277338</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.576531536291638</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.368336454051302</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.8325789171934</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.154349260156668</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.144877451159352</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.147476037454092</v>
       </c>
     </row>
@@ -1665,95 +1341,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.0625772201692652</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.116505436478945</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.35325139146675</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.575562395767317</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.402895113668335</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.516918809678844</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.886473974807497</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.201167318853901</v>
       </c>
     </row>
@@ -1778,95 +1427,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.59919028340081</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.255060728744939</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.999999999999995</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.715504978662871</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.907258064516129</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.326612903225806</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.229161113594648</v>
       </c>
     </row>
@@ -1891,95 +1513,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.696434129477608</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.705442383703247</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.490390189520623</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.447863247863246</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.260831159686995</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.285246835544318</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.288619115786948</v>
       </c>
     </row>
@@ -2004,95 +1599,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.657278968171417</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.17745995423341</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.500228832951944</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.509315581443729</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.334782608695654</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.939621781727045</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.358699779752411</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.094779946136451</v>
       </c>
     </row>
@@ -2117,95 +1685,68 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.515458449661513</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
         <v>0.99999999999995</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
         <v>0.999999999999968</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
         <v>0.844026805515887</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
         <v>0.999999999999972</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
         <v>0.449023462236327</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
         <v>0.124542124542125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
         <v>0.830698294656258</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rerun with v7 data
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -401,7 +401,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0896185966222548</v>
+        <v>0.158965320748276</v>
       </c>
     </row>
     <row r="3">
@@ -409,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0208619595159617</v>
+        <v>0.146962372110544</v>
       </c>
     </row>
     <row r="4">
@@ -417,7 +417,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.90258835020493</v>
+        <v>0.874193558521807</v>
       </c>
     </row>
     <row r="5">
@@ -425,7 +425,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.617880140186009</v>
+        <v>0.728339031091421</v>
       </c>
     </row>
     <row r="6">
@@ -433,7 +433,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.276767428792189</v>
+        <v>0.148792161026365</v>
       </c>
     </row>
     <row r="7">
@@ -441,7 +441,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.732449677492432</v>
+        <v>0.836515635385441</v>
       </c>
     </row>
     <row r="8">
@@ -449,7 +449,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.282133084993859</v>
+        <v>0.196307130417606</v>
       </c>
     </row>
     <row r="9">
@@ -457,7 +457,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.284369753577153</v>
+        <v>0.134720453987371</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.681940144478844</v>
+        <v>0.658978328173375</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.284829721362229</v>
+        <v>0.335913312693499</v>
       </c>
     </row>
     <row r="4">
@@ -511,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.508771929824559</v>
+        <v>0.201754385964909</v>
       </c>
     </row>
     <row r="6">
@@ -519,7 +519,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999999999999994</v>
+        <v>0.661919504643954</v>
       </c>
     </row>
     <row r="7">
@@ -527,7 +527,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.635364635364635</v>
+        <v>0.490842490842491</v>
       </c>
     </row>
     <row r="8">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0759240759240759</v>
+        <v>0.851814851814852</v>
       </c>
     </row>
     <row r="9">
@@ -543,7 +543,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.924520737821253</v>
+        <v>0.812910413930149</v>
       </c>
     </row>
   </sheetData>
@@ -629,7 +629,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.646990031211512</v>
+        <v>0.714399735860193</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.353287117317915</v>
+        <v>0.371730893209898</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.428523908344215</v>
+        <v>0.323012594134958</v>
       </c>
     </row>
   </sheetData>
@@ -887,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0600624085865772</v>
+        <v>0.0597088054740609</v>
       </c>
     </row>
   </sheetData>
@@ -973,7 +973,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.283319589457907</v>
+        <v>0.121982838921517</v>
       </c>
     </row>
   </sheetData>
@@ -1003,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0907981961597089</v>
+        <v>0.167077949858817</v>
       </c>
     </row>
     <row r="3">
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.426613045834412</v>
+        <v>0.383195002994785</v>
       </c>
     </row>
     <row r="5">
@@ -1027,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.81427569093866</v>
+        <v>0.613074356122186</v>
       </c>
     </row>
     <row r="6">
@@ -1035,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.780633752602614</v>
+        <v>0.744072711369706</v>
       </c>
     </row>
     <row r="7">
@@ -1043,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.878298596491423</v>
+        <v>0.750771130026087</v>
       </c>
     </row>
     <row r="8">
@@ -1051,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.759361447436373</v>
+        <v>0.873790272564862</v>
       </c>
     </row>
     <row r="9">
@@ -1059,7 +1059,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.739996268959378</v>
+        <v>0.342330077926341</v>
       </c>
     </row>
   </sheetData>
@@ -1089,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.713705357283287</v>
+        <v>0.178765281671919</v>
       </c>
     </row>
     <row r="3">
@@ -1097,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.818370221050665</v>
       </c>
     </row>
     <row r="4">
@@ -1105,7 +1105,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.987141116454481</v>
+        <v>0.946079289753066</v>
       </c>
     </row>
     <row r="5">
@@ -1113,7 +1113,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.946801804848752</v>
+        <v>0.971915975844798</v>
       </c>
     </row>
     <row r="6">
@@ -1121,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.639519327674786</v>
+        <v>0.399888854575204</v>
       </c>
     </row>
     <row r="7">
@@ -1129,7 +1129,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00369227398780271</v>
+        <v>0.00307470546413358</v>
       </c>
     </row>
     <row r="8">
@@ -1137,7 +1137,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0034650073118416</v>
+        <v>0.00261898965050277</v>
       </c>
     </row>
     <row r="9">
@@ -1145,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0878796824057952</v>
+        <v>0.0235346934986866</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1175,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.498965426816437</v>
+        <v>0.686514723206952</v>
       </c>
     </row>
     <row r="3">
@@ -1183,7 +1183,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0565098418868229</v>
+        <v>0.0187897276984035</v>
       </c>
     </row>
     <row r="4">
@@ -1191,7 +1191,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.999999999999979</v>
+        <v>0.999999999999969</v>
       </c>
     </row>
     <row r="5">
@@ -1199,7 +1199,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.631203160659328</v>
+        <v>0.498680101486856</v>
       </c>
     </row>
     <row r="6">
@@ -1207,7 +1207,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999999999999973</v>
+        <v>0.999999999999936</v>
       </c>
     </row>
     <row r="7">
@@ -1215,7 +1215,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.23832192708036</v>
+        <v>0.164184087571725</v>
       </c>
     </row>
     <row r="8">
@@ -1223,7 +1223,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.419110881762562</v>
+        <v>0.206137365005419</v>
       </c>
     </row>
     <row r="9">
@@ -1231,7 +1231,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.167425229268679</v>
+        <v>0.183607803413947</v>
       </c>
     </row>
   </sheetData>
@@ -1261,7 +1261,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.233152960277338</v>
+        <v>0.106717016062028</v>
       </c>
     </row>
     <row r="3">
@@ -1269,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.765661101678121</v>
       </c>
     </row>
     <row r="4">
@@ -1277,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.576531536291638</v>
+        <v>0.474483025747333</v>
       </c>
     </row>
     <row r="5">
@@ -1285,7 +1285,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.368336454051302</v>
+        <v>0.293332234357925</v>
       </c>
     </row>
     <row r="6">
@@ -1293,7 +1293,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8325789171934</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.154349260156668</v>
+        <v>0.194785106832606</v>
       </c>
     </row>
     <row r="8">
@@ -1309,7 +1309,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.144877451159352</v>
+        <v>0.0979396497170013</v>
       </c>
     </row>
     <row r="9">
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.147476037454092</v>
+        <v>0.429688254318136</v>
       </c>
     </row>
   </sheetData>
@@ -1347,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0625772201692652</v>
+        <v>0.19955781429289</v>
       </c>
     </row>
     <row r="3">
@@ -1355,7 +1355,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.116505436478945</v>
+        <v>0.309865431987481</v>
       </c>
     </row>
     <row r="4">
@@ -1363,7 +1363,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.35325139146675</v>
+        <v>0.248632198653321</v>
       </c>
     </row>
     <row r="5">
@@ -1371,7 +1371,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.575562395767317</v>
+        <v>0.0735420797512746</v>
       </c>
     </row>
     <row r="6">
@@ -1379,7 +1379,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.402895113668335</v>
+        <v>0.276011201785736</v>
       </c>
     </row>
     <row r="7">
@@ -1387,7 +1387,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.516918809678844</v>
+        <v>0.155730714345813</v>
       </c>
     </row>
     <row r="8">
@@ -1395,7 +1395,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.886473974807497</v>
+        <v>0.482383043352823</v>
       </c>
     </row>
     <row r="9">
@@ -1403,7 +1403,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.201167318853901</v>
+        <v>0.331349500657068</v>
       </c>
     </row>
   </sheetData>
@@ -1433,7 +1433,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.59919028340081</v>
+        <v>0.737839053628527</v>
       </c>
     </row>
     <row r="3">
@@ -1441,7 +1441,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.255060728744939</v>
+        <v>0.63088594667542</v>
       </c>
     </row>
     <row r="4">
@@ -1449,7 +1449,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.999999999999995</v>
+        <v>0.751066856330015</v>
       </c>
     </row>
     <row r="5">
@@ -1457,7 +1457,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.715504978662871</v>
+        <v>0.300616405879564</v>
       </c>
     </row>
     <row r="6">
@@ -1465,7 +1465,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.363411994990942</v>
       </c>
     </row>
     <row r="7">
@@ -1473,7 +1473,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.907258064516129</v>
+        <v>0.668548387096774</v>
       </c>
     </row>
     <row r="8">
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.326612903225806</v>
+        <v>0.0701612903225806</v>
       </c>
     </row>
     <row r="9">
@@ -1489,7 +1489,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.229161113594648</v>
+        <v>0.519033579392551</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1575,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.288619115786948</v>
+        <v>0.150045324913797</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.657278968171417</v>
+        <v>0.406344451378776</v>
       </c>
     </row>
     <row r="3">
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.17745995423341</v>
+        <v>0.080976353928299</v>
       </c>
     </row>
     <row r="4">
@@ -1621,7 +1621,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.500228832951944</v>
+        <v>0.480877424126851</v>
       </c>
     </row>
     <row r="5">
@@ -1629,7 +1629,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.509315581443729</v>
+        <v>0.270560062871274</v>
       </c>
     </row>
     <row r="6">
@@ -1637,7 +1637,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.334782608695654</v>
+        <v>0.388985507246377</v>
       </c>
     </row>
     <row r="7">
@@ -1645,7 +1645,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.939621781727045</v>
+        <v>0.914425100183614</v>
       </c>
     </row>
     <row r="8">
@@ -1653,7 +1653,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.358699779752411</v>
+        <v>0.640665835712275</v>
       </c>
     </row>
     <row r="9">
@@ -1661,7 +1661,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.094779946136451</v>
+        <v>0.158298398203477</v>
       </c>
     </row>
   </sheetData>
@@ -1691,7 +1691,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.515458449661513</v>
+        <v>0.285789423282333</v>
       </c>
     </row>
     <row r="3">
@@ -1699,7 +1699,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.99999999999995</v>
+        <v>0.760344776517266</v>
       </c>
     </row>
     <row r="4">
@@ -1707,7 +1707,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.999999999999968</v>
+        <v>0.999999999999994</v>
       </c>
     </row>
     <row r="5">
@@ -1715,7 +1715,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.844026805515887</v>
+        <v>0.870022337929905</v>
       </c>
     </row>
     <row r="6">
@@ -1723,7 +1723,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.999999999999972</v>
+        <v>0.999999999999997</v>
       </c>
     </row>
     <row r="7">
@@ -1731,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.449023462236327</v>
+        <v>0.4606509551112</v>
       </c>
     </row>
     <row r="8">
@@ -1739,7 +1739,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.124542124542125</v>
+        <v>0.291184371184371</v>
       </c>
     </row>
     <row r="9">
@@ -1747,7 +1747,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.830698294656258</v>
+        <v>0.823354276121646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun with updated histologies
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -401,7 +401,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.158965320748276</v>
+        <v>0.258370854717028</v>
       </c>
     </row>
     <row r="3">
@@ -409,7 +409,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.146962372110544</v>
+        <v>0.1408182448886</v>
       </c>
     </row>
     <row r="4">
@@ -417,7 +417,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.874193558521807</v>
+        <v>0.830977487111851</v>
       </c>
     </row>
     <row r="5">
@@ -425,7 +425,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.728339031091421</v>
+        <v>0.661238327317944</v>
       </c>
     </row>
     <row r="6">
@@ -433,7 +433,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.148792161026365</v>
+        <v>0.143818354993677</v>
       </c>
     </row>
     <row r="7">
@@ -441,7 +441,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.836515635385441</v>
+        <v>0.868300106934329</v>
       </c>
     </row>
     <row r="8">
@@ -449,7 +449,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.196307130417606</v>
+        <v>0.148440568057781</v>
       </c>
     </row>
     <row r="9">
@@ -457,7 +457,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.134720453987371</v>
+        <v>0.232016027318013</v>
       </c>
     </row>
   </sheetData>
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.335913312693499</v>
+        <v>0.335913312693498</v>
       </c>
     </row>
     <row r="4">
@@ -543,7 +543,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.812910413930149</v>
+        <v>0.880504238997841</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.297702297702298</v>
+        <v>0.43956043956044</v>
       </c>
     </row>
     <row r="3">
@@ -605,7 +605,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.604395604395606</v>
+        <v>0.571428571428572</v>
       </c>
     </row>
     <row r="7">
@@ -613,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.503496503496504</v>
+        <v>0.373626373626374</v>
       </c>
     </row>
     <row r="8">
@@ -621,7 +621,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.33006993006993</v>
+        <v>0.23976023976024</v>
       </c>
     </row>
     <row r="9">
@@ -629,7 +629,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.714399735860193</v>
+        <v>0.394496316665903</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +659,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.533238741934394</v>
+        <v>0.708636291244987</v>
       </c>
     </row>
     <row r="3">
@@ -667,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.408212560386474</v>
+        <v>0.685990338164251</v>
       </c>
     </row>
     <row r="4">
@@ -675,7 +675,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.282003986351813</v>
+        <v>0.227445018749371</v>
       </c>
     </row>
     <row r="5">
@@ -683,7 +683,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.615904868078785</v>
+        <v>0.522998740390055</v>
       </c>
     </row>
     <row r="6">
@@ -691,7 +691,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.231809736157562</v>
+        <v>0.120821207777732</v>
       </c>
     </row>
     <row r="7">
@@ -699,7 +699,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.367632367632368</v>
+        <v>0.417317976141506</v>
       </c>
     </row>
     <row r="8">
@@ -707,7 +707,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.635364635364635</v>
+        <v>0.600884409707939</v>
       </c>
     </row>
     <row r="9">
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.371730893209898</v>
+        <v>0.530489581031042</v>
       </c>
     </row>
   </sheetData>
@@ -1059,7 +1059,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.342330077926341</v>
+        <v>0.446428676155261</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0235346934986866</v>
+        <v>0.0243140925220621</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1231,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.183607803413947</v>
+        <v>0.434462529964249</v>
       </c>
     </row>
   </sheetData>
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.429688254318136</v>
+        <v>0.33110233659148</v>
       </c>
     </row>
   </sheetData>
@@ -1403,7 +1403,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.331349500657068</v>
+        <v>0.589401718172365</v>
       </c>
     </row>
   </sheetData>
@@ -1489,7 +1489,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.519033579392551</v>
+        <v>0.882365751773955</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1575,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.150045324913797</v>
+        <v>0.160726716942899</v>
       </c>
     </row>
   </sheetData>
@@ -1661,7 +1661,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.158298398203477</v>
+        <v>0.521993004459526</v>
       </c>
     </row>
   </sheetData>
@@ -1747,7 +1747,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.823354276121646</v>
+        <v>0.824214113519518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun with NF1 intronic plp
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -457,7 +457,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.232016027318013</v>
+        <v>0.295225120835944</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.43956043956044</v>
+        <v>0.225641025641026</v>
       </c>
     </row>
     <row r="3">
@@ -589,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.589743589743591</v>
       </c>
     </row>
     <row r="5">
@@ -597,7 +597,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.589743589743591</v>
       </c>
     </row>
     <row r="6">
@@ -605,7 +605,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.571428571428572</v>
+        <v>0.476190476190476</v>
       </c>
     </row>
     <row r="7">
@@ -613,7 +613,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.373626373626374</v>
+        <v>0.456043956043956</v>
       </c>
     </row>
     <row r="8">
@@ -621,7 +621,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.23976023976024</v>
+        <v>0.291208791208791</v>
       </c>
     </row>
     <row r="9">
@@ -1059,7 +1059,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.446428676155261</v>
+        <v>0.672416118643011</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0243140925220621</v>
+        <v>0.0114236813806622</v>
       </c>
     </row>
   </sheetData>
@@ -1231,7 +1231,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.434462529964249</v>
+        <v>0.47293154793839</v>
       </c>
     </row>
   </sheetData>
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.33110233659148</v>
+        <v>0.233368156730013</v>
       </c>
     </row>
   </sheetData>
@@ -1403,7 +1403,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.589401718172365</v>
+        <v>0.840678123585337</v>
       </c>
     </row>
   </sheetData>
@@ -1489,7 +1489,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.882365751773955</v>
+        <v>0.434874810217698</v>
       </c>
     </row>
   </sheetData>
@@ -1747,7 +1747,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.824214113519518</v>
+        <v>0.762129815426868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun modules with metastatic secondary samples removed
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -457,7 +457,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.295225120835944</v>
+        <v>0.250282533354947</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.658978328173375</v>
+        <v>0.391296869625043</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.335913312693498</v>
+        <v>0.602683178534572</v>
       </c>
     </row>
     <row r="4">
@@ -511,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.201754385964909</v>
+        <v>0.154798761609906</v>
       </c>
     </row>
     <row r="6">
@@ -519,7 +519,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.661919504643954</v>
+        <v>0.647832817337455</v>
       </c>
     </row>
     <row r="7">
@@ -527,7 +527,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.490842490842491</v>
+        <v>0.724164724164724</v>
       </c>
     </row>
     <row r="8">
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.851814851814852</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -543,7 +543,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.880504238997841</v>
+        <v>0.285074392719691</v>
       </c>
     </row>
   </sheetData>
@@ -1003,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.167077949858817</v>
+        <v>0.197752682100508</v>
       </c>
     </row>
     <row r="3">
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.383195002994785</v>
+        <v>0.272772444946358</v>
       </c>
     </row>
     <row r="5">
@@ -1027,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.613074356122186</v>
+        <v>0.719446640316208</v>
       </c>
     </row>
     <row r="6">
@@ -1035,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.744072711369706</v>
+        <v>0.23399209486166</v>
       </c>
     </row>
     <row r="7">
@@ -1043,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>0.750771130026087</v>
+        <v>0.606281774296427</v>
       </c>
     </row>
     <row r="8">
@@ -1051,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.873790272564862</v>
+        <v>0.962630010490645</v>
       </c>
     </row>
     <row r="9">
@@ -1059,7 +1059,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.672416118643011</v>
+        <v>0.907180398931276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rerun with GPR161 typo corrected
</commit_message>
<xml_diff>
--- a/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
+++ b/analyses/demo-clin-stats/results/demo-clin-pvalues-by-histology.xlsx
@@ -1089,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>0.178765281671919</v>
+        <v>0.099269066823374</v>
       </c>
     </row>
     <row r="3">
@@ -1097,7 +1097,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>0.818370221050665</v>
+        <v>0.647110170368091</v>
       </c>
     </row>
     <row r="4">
@@ -1105,7 +1105,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>0.946079289753066</v>
+        <v>0.976232230683878</v>
       </c>
     </row>
     <row r="5">
@@ -1113,7 +1113,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>0.971915975844798</v>
+        <v>0.950212628821588</v>
       </c>
     </row>
     <row r="6">
@@ -1121,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.399888854575204</v>
+        <v>0.410362840774718</v>
       </c>
     </row>
     <row r="7">

</xml_diff>